<commit_message>
new files, upd proguru
</commit_message>
<xml_diff>
--- a/proguru.xlsx
+++ b/proguru.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Slava\Desktop\proger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B51A1F-B5F1-4FB0-9AC9-0FE7464F4A8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D48A39-807C-48CF-9E8A-8EB208A7EB21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7410" yWindow="135" windowWidth="23640" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Правила вывода и скриншоты" sheetId="1" r:id="rId1"/>
+    <sheet name="Таблица тестов" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="52">
   <si>
     <t>Репутация</t>
   </si>
@@ -87,9 +88,6 @@
     <t>да</t>
   </si>
   <si>
-    <t>жа</t>
-  </si>
-  <si>
     <t>сильный</t>
   </si>
   <si>
@@ -121,6 +119,69 @@
   </si>
   <si>
     <t>Уровень</t>
+  </si>
+  <si>
+    <t>Оценка коллег</t>
+  </si>
+  <si>
+    <t>Студент?</t>
+  </si>
+  <si>
+    <t>Ср.бал</t>
+  </si>
+  <si>
+    <t>кол-во прод.пр.</t>
+  </si>
+  <si>
+    <t>кол-во законч.пр.</t>
+  </si>
+  <si>
+    <t>квалификация</t>
+  </si>
+  <si>
+    <t>результат работы</t>
+  </si>
+  <si>
+    <t>опыт</t>
+  </si>
+  <si>
+    <t>уровень</t>
+  </si>
+  <si>
+    <t>Низкая</t>
+  </si>
+  <si>
+    <t>Высокая</t>
+  </si>
+  <si>
+    <t>Нет</t>
+  </si>
+  <si>
+    <t>Не студент</t>
+  </si>
+  <si>
+    <t>Высокий</t>
+  </si>
+  <si>
+    <t>Средний</t>
+  </si>
+  <si>
+    <t>Низкий</t>
+  </si>
+  <si>
+    <t>Маленький</t>
+  </si>
+  <si>
+    <t>Да</t>
+  </si>
+  <si>
+    <t>Сильный</t>
+  </si>
+  <si>
+    <t>Большой</t>
+  </si>
+  <si>
+    <t>Слабый</t>
   </si>
 </sst>
 </file>
@@ -136,7 +197,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,6 +219,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -189,13 +268,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -219,21 +301,21 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>14654</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>429722</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:colOff>439247</xdr:colOff>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>14464</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Рисунок 1">
+        <xdr:cNvPr id="8" name="Рисунок 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{261BF11D-4081-4464-B732-3C45DF4A0280}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B140D43-A4ED-4B62-9FB9-4330A16BAEE0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -250,7 +332,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="4777154"/>
-          <a:ext cx="2942857" cy="1523810"/>
+          <a:ext cx="2944322" cy="1523810"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -263,21 +345,21 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>586153</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>87924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>23060</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>575510</xdr:colOff>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>78210</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2">
+        <xdr:cNvPr id="9" name="Рисунок 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9F1A7D2-383B-4D22-A264-EB430C60C5B7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{633B40A0-D849-4D54-BE17-0ECA02BA94AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -293,8 +375,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7766538" y="6755424"/>
-          <a:ext cx="3085714" cy="1514286"/>
+          <a:off x="7768003" y="6755424"/>
+          <a:ext cx="3094507" cy="1514286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -307,21 +389,21 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>183173</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>307302</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>40078</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Рисунок 3">
+        <xdr:cNvPr id="10" name="Рисунок 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEA39011-D4A1-4E42-9E96-94A4E57EE7C2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CA5D87B-AAB1-422F-BCA0-8FCC92C46844}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -338,7 +420,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="6469673"/>
-          <a:ext cx="3428571" cy="1761905"/>
+          <a:ext cx="3431502" cy="1761905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -350,22 +432,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>249117</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>146539</xdr:rowOff>
+      <xdr:colOff>256444</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95252</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>560041</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>165372</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>167318</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>114085</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Рисунок 5">
+        <xdr:cNvPr id="11" name="Рисунок 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82EA4E8F-0A48-4730-9E25-6883049F914F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76CD745E-9443-4325-9DED-43A4933B844B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -381,8 +463,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3370386" y="4718539"/>
-          <a:ext cx="3761905" cy="1733333"/>
+          <a:off x="3380644" y="4667252"/>
+          <a:ext cx="3758974" cy="1733333"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -394,22 +476,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>256441</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>109903</xdr:rowOff>
+      <xdr:colOff>197826</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>80595</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>596720</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>176355</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>480955</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>147047</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Рисунок 6">
+        <xdr:cNvPr id="12" name="Рисунок 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F52F3B3-A835-4476-B902-BFF05081EFB4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECCDEC09-623D-4EE6-9A53-8C4E87285A14}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -425,8 +507,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7436826" y="4681903"/>
-          <a:ext cx="3380952" cy="1780952"/>
+          <a:off x="7379676" y="4652595"/>
+          <a:ext cx="3388279" cy="1780952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -438,22 +520,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>586153</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>36635</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>307989</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>56929</xdr:rowOff>
+      <xdr:colOff>502885</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>93564</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Рисунок 7">
+        <xdr:cNvPr id="13" name="Рисунок 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3867ED1D-722E-4B01-BF55-A1A594DABEEF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E67F3C28-875A-49CF-9FFA-3D0E2F569F34}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -469,8 +551,184 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3707422" y="6477000"/>
-          <a:ext cx="3780952" cy="1771429"/>
+          <a:off x="3695699" y="6513635"/>
+          <a:ext cx="3779486" cy="1771429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>183173</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95582</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>59149</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Рисунок 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7701FF1-2446-495C-BDCD-3060A9E1F3F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7327" y="8565173"/>
+          <a:ext cx="3212455" cy="1590476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>446943</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>919852</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Рисунок 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6D830BC-3BDF-4914-9EE0-5740493A539A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3571143" y="8572500"/>
+          <a:ext cx="3273259" cy="1676190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>241789</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>109904</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>43523</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>62047</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Рисунок 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA1ECFC1-2A9B-4097-916D-6A492D47C540}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7224347" y="6396404"/>
+          <a:ext cx="3516484" cy="1857143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>29307</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>161191</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>291199</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>160977</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Рисунок 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{378431E6-02A1-4B32-AEBB-E7D2C0B2EDE5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11334749" y="6447691"/>
+          <a:ext cx="3302565" cy="1714286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -747,9 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="23" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,7 +1136,7 @@
         <v>7</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -891,13 +1148,13 @@
         <v>18</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -905,19 +1162,19 @@
         <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -925,39 +1182,39 @@
         <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -968,29 +1225,29 @@
         <v>8</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -998,26 +1255,26 @@
         <v>18</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="E17" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.25">
       <c r="E18" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>3</v>
@@ -1028,7 +1285,7 @@
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.25">
       <c r="E19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>3</v>
@@ -1039,29 +1296,29 @@
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.25">
       <c r="E20" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.25">
       <c r="E21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="4:8" x14ac:dyDescent="0.25">
       <c r="E22" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>4</v>
@@ -1072,7 +1329,7 @@
     </row>
     <row r="23" spans="4:8" x14ac:dyDescent="0.25">
       <c r="E23" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>4</v>
@@ -1104,6 +1361,446 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEAA3945-6131-42FF-A059-74F249BA3931}">
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>